<commit_message>
This is a mern stact project
</commit_message>
<xml_diff>
--- a/backend/income_details.xlsx
+++ b/backend/income_details.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,47 +416,55 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Factory</v>
+        <v>salary</v>
       </c>
       <c r="C2" s="1">
-        <v>45845.66033196759</v>
+        <v>45846.59566582176</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Trading</v>
+        <v>Factory</v>
       </c>
       <c r="C3" s="1">
-        <v>45844.6799502662</v>
+        <v>45845.66033196759</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>saving money</v>
+        <v>Trading</v>
       </c>
       <c r="C4" s="1">
-        <v>45844.67518486111</v>
+        <v>45844.6799502662</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Interest From Saving Account</v>
+        <v>saving money</v>
       </c>
       <c r="C5" s="1">
-        <v>45841.76753356482</v>
+        <v>45844.67518486111</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
+        <v>Interest From Saving Account</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45841.76753356482</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
         <v>Salary</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C7" s="1">
         <v>45810.675252395835</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>